<commit_message>
added SAUP SSP plot
</commit_message>
<xml_diff>
--- a/tables/Table1_final_depletion_priors.xlsx
+++ b/tables/Table1_final_depletion_priors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/com_review/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B41BF8F-F986-8346-878F-1C59F8148DD5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141E6300-334C-464C-A9D9-46929212203A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="460" windowWidth="25040" windowHeight="14500" xr2:uid="{30EEEBCE-3399-534B-A3CA-6D621B793149}"/>
   </bookViews>
@@ -591,7 +591,7 @@
   <dimension ref="A2:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>